<commit_message>
feat: apply review feedback
</commit_message>
<xml_diff>
--- a/examples/target-audiences.xlsx
+++ b/examples/target-audiences.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{340A8779-436A-484A-B045-888BA4291848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsaplin/Work/Sources/aem-genai-assistant/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B5AA90-D98B-5B47-92F1-1E78932A4055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="30580" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Universal audience</t>
   </si>
@@ -115,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +183,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -236,20 +241,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{84672798-42E7-49D9-A283-5DF7DF6C95B3}" name="Table2" displayName="Table2" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B13" xr:uid="{84672798-42E7-49D9-A283-5DF7DF6C95B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{84672798-42E7-49D9-A283-5DF7DF6C95B3}" name="Table2" displayName="Table2" ref="A1:B12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CEF662C1-8803-4CB9-90A4-96F6741599DE}" name="Key" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A93858D9-7BCB-4883-BCB4-2899C25A723F}" name="Value" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CEF662C1-8803-4CB9-90A4-96F6741599DE}" name="Key" headerRowDxfId="0" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A93858D9-7BCB-4883-BCB4-2899C25A723F}" name="Value" headerRowDxfId="1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -287,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -393,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -535,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,44 +547,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="91.140625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="57.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60.75">
+    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45.75">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="38.25">
+    <row r="4" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -588,7 +592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="37.5" customHeight="1">
+    <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -596,15 +600,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="25.5">
+    <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5">
+    <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -612,7 +616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="38.25">
+    <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -620,7 +624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25">
+    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -628,7 +632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="38.25">
+    <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -636,60 +640,52 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="25.5">
+    <row r="11" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="38.25">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="38.25">
-      <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="E14" s="6"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="E16" s="6"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="6"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="6"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="6"/>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="6"/>
-    </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="6"/>
-    </row>
-    <row r="28" spans="5:5">
-      <c r="E28" s="6"/>
-    </row>
-    <row r="30" spans="5:5">
-      <c r="E30" s="6"/>
-    </row>
-    <row r="32" spans="5:5">
-      <c r="E32" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: reading and writing prompts using settings api (#204)
</commit_message>
<xml_diff>
--- a/examples/target-audiences.xlsx
+++ b/examples/target-audiences.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{340A8779-436A-484A-B045-888BA4291848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsaplin/Work/Sources/aem-genai-assistant/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B5AA90-D98B-5B47-92F1-1E78932A4055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="30580" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Universal audience</t>
   </si>
@@ -115,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +183,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -236,20 +241,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{84672798-42E7-49D9-A283-5DF7DF6C95B3}" name="Table2" displayName="Table2" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B13" xr:uid="{84672798-42E7-49D9-A283-5DF7DF6C95B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{84672798-42E7-49D9-A283-5DF7DF6C95B3}" name="Table2" displayName="Table2" ref="A1:B12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CEF662C1-8803-4CB9-90A4-96F6741599DE}" name="Key" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A93858D9-7BCB-4883-BCB4-2899C25A723F}" name="Value" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CEF662C1-8803-4CB9-90A4-96F6741599DE}" name="Key" headerRowDxfId="0" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A93858D9-7BCB-4883-BCB4-2899C25A723F}" name="Value" headerRowDxfId="1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -287,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -393,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -535,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,44 +547,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="91.140625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="57.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60.75">
+    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45.75">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="38.25">
+    <row r="4" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -588,7 +592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="37.5" customHeight="1">
+    <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -596,15 +600,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="25.5">
+    <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5">
+    <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -612,7 +616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="38.25">
+    <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -620,7 +624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25">
+    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -628,7 +632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="38.25">
+    <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -636,60 +640,52 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="25.5">
+    <row r="11" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="38.25">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="39" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="38.25">
-      <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="E14" s="6"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="E16" s="6"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="6"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="6"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="6"/>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="6"/>
-    </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="6"/>
-    </row>
-    <row r="28" spans="5:5">
-      <c r="E28" s="6"/>
-    </row>
-    <row r="30" spans="5:5">
-      <c r="E30" s="6"/>
-    </row>
-    <row r="32" spans="5:5">
-      <c r="E32" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>